<commit_message>
added code for nn input(observation + command(lin vel + ang quat pos))
</commit_message>
<xml_diff>
--- a/trains_et_procedures.xlsx
+++ b/trains_et_procedures.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
   <si>
     <t xml:space="preserve">motion_imitation_base/ : architecture du réseau de neurones de l'article (commande avec prédiction motion capture comme référence)
 motion_imitation/ : architecture du réseau de neurones avec commande en vitesse (vitesse linéaire + angulaire)</t>
@@ -35,7 +35,13 @@
     <t xml:space="preserve">Commentaires</t>
   </si>
   <si>
-    <t xml:space="preserve">Procédure de lancement</t>
+    <t xml:space="preserve">Procédure de lancement (test) voir modèle sur le git et descriptif des args ci-dessus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procédure de lancement (train) voir modèle sur le git et descriptif des args ci-dessus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code de base (architecture de base) : le dossier du projet est : motion_imitation_base/</t>
   </si>
   <si>
     <t xml:space="preserve">dog pace base</t>
@@ -44,7 +50,7 @@
     <t xml:space="preserve">motion_imitation/data/motions/dog_pace.txt</t>
   </si>
   <si>
-    <t xml:space="preserve">motion_imitation_base/data/policies/dog_pace.zip</t>
+    <t xml:space="preserve">motion_imitation/data/policies/dog_pace.zip</t>
   </si>
   <si>
     <t xml:space="preserve">modèle déjà entraîné compris dans le repository de base de l’article</t>
@@ -54,10 +60,13 @@
 motion_imitation_base</t>
   </si>
   <si>
+    <t xml:space="preserve">commande mpi_exec (voir page git)</t>
+  </si>
+  <si>
     <t xml:space="preserve">temoin_plat</t>
   </si>
   <si>
-    <t xml:space="preserve">motion/imitation_base/model_saves/temoin_plat.zip</t>
+    <t xml:space="preserve">model_saves/temoin_plat.zip</t>
   </si>
   <si>
     <t xml:space="preserve">réplique des résultats de l’article</t>
@@ -69,7 +78,7 @@
     <t xml:space="preserve">marche terrain escarpée</t>
   </si>
   <si>
-    <t xml:space="preserve">motion_imitation_base/model_saves/rugged_terrain.zip</t>
+    <t xml:space="preserve">model_saves/rugged_terrain.zip</t>
   </si>
   <si>
     <t xml:space="preserve">robot marchant sur un terrain accidenté (petites bosses)</t>
@@ -78,8 +87,8 @@
     <t xml:space="preserve">décommenter bloc à la ligne 225 de motion_imitation/envs/locomotion_gym_env.py et commenter ligne 258-260 (terrain plat)</t>
   </si>
   <si>
-    <t xml:space="preserve">Ajouter / Enlever le bruit de commande :
-Ajouter / Enlever le yaw et yaw rate dans l'entrée du réseau :</t>
+    <t xml:space="preserve">commande mpi_exec (voir page git)
+motion_imitation/envs/locomotion_gym_env.py et commenter ligne 258-260 (terrain plat)</t>
   </si>
   <si>
     <t xml:space="preserve">A partir d'ici l'architecture du réseau a été modifiée pour avoir une commande en vitesse en entrée. Le dossier du projet est : motion_imitation/</t>
@@ -100,13 +109,185 @@
 Commenter les fonctions : build_target_obs() dans le même fichier ligne 266 et ligne 294. Faire de même pour les fonctions get_target_obs_bounds() ligne 341 et ligne 371.</t>
   </si>
   <si>
+    <t xml:space="preserve">slurm_script : bash sbatch_script.sh, changer la commande mpi_exec du fichier motion_imi.job en fonction (model file, ref file, etc.)
+Décommenter et commenter les mêmes lignes que pour un test</t>
+  </si>
+  <si>
     <t xml:space="preserve">inverted_reward</t>
   </si>
   <si>
-    <t xml:space="preserve">marche ligne droite </t>
+    <t xml:space="preserve">model_saves/inverted_reward/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marche ligne droite avec les coefficients des sous-rewards pose_weight et root_pose_weight inversés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test.sh
+Calcul du reward se trouvant dans motion_imitation/envs/env_wrappers/imitation_task.py ligne 409
+Commenter tous les blocs sauf celui commenté par "reward inversé"</t>
   </si>
   <si>
     <t xml:space="preserve">tweaked_reward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/tweaked_reward/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marche ligne droite avec les coefficients des sous-rewards modifiés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test.sh
+Calcul du reward se trouvant dans motion_imitation/envs/env_wrappers/imitation_task.py ligne 409
+Commenter tous les blocs sauf celui commenté par "reward modifié"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idem mais avec le script de lancement d'un train : bash sbatch_script.sh et modification de motion_imi.job en conséquence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">custom_ref_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/data/motions/data_train_xx.txt (data_train_1 to 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/custom_ref_test/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">premiers tests avec une référence custom, différente du fichier dog_pace.txt.
+Mauvais résultats : angles de simulation matlab non accordables avec les angles acceptés par Pybullet (modulo 2pi)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test.sh avec les bons arguments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mpi_exec.sh ou sbatch_script / motion_imi.job avec bons arguments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmd_noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/data/motions/data_train_4.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/cmd_noise/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marche ligne droite avec start/stop + commande bruitée </t>
+  </si>
+  <si>
+    <t xml:space="preserve">test.sh
+Lors du test, c'est mieux d'enlever le bruit (n'est utile que pour l'entrainement) : Commenter motion_imitation/envs/env_wrappers/imitation_wrapper_env.py ligne 117, décommenter ligne 118.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mpi_train.sh / slurm script
+Ajouter le bruit à la commande : Décommenter motion_imitation/envs/env_wrappers/imitation_wrapper_env.py ligne 117, commenter ligne 118.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hard reference no yaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/data/motions/data_train_7.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/hard_ref_noyaw/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marche avec une référence compliquée pour apprendre la marche arrière + changement de directions.
+Version sans la mesure du yaw et yaw rate en entrée du réseau. Mauvais résultats, ne marche pas pour le réseau retrain, marche "mal" vers l'avant quand la ref avance en ligne droite vers l'avant (réseau train from scratch)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test.sh avec l'observation classique (r,p,dr,dp) : Décommenter motion_imitation/envs/env_builder.py ligne 98 et commenter la ligne 97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mpi_train.sh / sbatch_script – motion_imi.job avec l'observation classique (r,p,dr,dp) : Décommenter motion_imitation/envs/env_builder.py ligne 98 et commenter la ligne 97. Ajout du noise (cf. cmd_noise).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hard reference with yaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/hard_ref_yaw/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marche avec une référence compliquée pour apprendre la marche arrière + changement de directions.
+Version avec la mesure du yaw et yaw rate en entrée du réseau. Mauvais résultats.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test.sh avec l'observation avec le yaw (r,p,y,dr,dp,dy) : Commenter motion_imitation/envs/env_builder.py ligne 98 et décommenter la ligne 97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mpi_train.sh / sbatch_script – motion_imi.job avec l'observation avec le yaw (r,p,y,dr,dp,dy) : Commenter motion_imitation/envs/env_builder.py ligne 98 et décommenter la ligne 97. Ajout du noise (cf. cmd_noise).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yaw observation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/yaw_obs/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marche ligne droite start/stop + yaw &amp; yaw rate dans l'observation. Meilleurs résultats : yaw_obs_130M.zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test.sh avec l'observation avec le yaw (r,p,y,dr,dp,dy) : Commenter motion_imitation/envs/env_builder.py ligne 98 et décommenter la ligne 97.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zigzag_noyaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/data/motions/data_train_8.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/zigzag_noyaw/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marche en zigzag sans vitesse sur le yaw (garde un cap constant, pas de cotés). Mauvais résultats : dérive plus importante et allure de marche mauvaise : marche en sautillant.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zigzag_yaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/data/motions/data_train_9.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/zigzag_yaw/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marche en zigzag avec vitesse sur le yaw (cap changeant, pas de pas cotés). Mauvais résultats : marche quasi rectiligne, ne suit pas la référence qui marche en zigzagant du tout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">static_turn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/data/motions/data_train_13.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/static_turn/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marche où le robot tourne autour de lui-même (à partir d'un fichier .txt de ref custom). Mauvais résultats : robot reste immobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test.sh : obs avec le yaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mpi_train.sh / sbatch_script – motion_imi.job obs avec le yaw. Ajout du noise pour le train.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/data/motions/dog_spin.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/spin/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marche où le robot tourne (assez vite) autour de lui-même (fichier de ref txt non custom : déjà présent dans le git)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test.sh : obs avec le yaw + commande changée : à la place de donner la commande en vitesse des vitesses angulaires (dr, dp, dy) on donne la position angulaire à rejoindre via un quaternion (qx,qy,qz,qw) : Décommenter fonction build_target_obs() ligne 266 de motion_imitation/envs/env_wrappers/imitation_task.py et commenter les deux autres (autres cas) + faire de meme pour la fonction get_target_obs_bounds() du meme fichier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mpi_train.sh /sbatch_script – motion_imi.job : obs avec le yaw + commande changée : à la place de donner la commande en vitesse des vitesses angulaires (dr, dp, dy) on donne la position angulaire à rejoindre via un quaternion (qx,qy,qz,qw) : Décommenter fonction build_target_obs() ligne 266 de motion_imitation/envs/env_wrappers/imitation_task.py et commenter les deux autres (autres cas) + faire de meme pour la fonction get_target_obs_bounds() du meme fichier.</t>
   </si>
 </sst>
 </file>
@@ -156,12 +337,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA6A6"/>
+        <bgColor rgb="FFFFCC99"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -208,7 +395,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -238,6 +425,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -255,6 +458,66 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFFA6A6"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -269,9 +532,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3232080</xdr:colOff>
+      <xdr:colOff>2955960</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>2503080</xdr:rowOff>
+      <xdr:rowOff>2502720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -285,7 +548,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="2154600"/>
-          <a:ext cx="12817800" cy="2260800"/>
+          <a:ext cx="12816720" cy="2260440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -306,9 +569,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1873800</xdr:colOff>
+      <xdr:colOff>1873440</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>232560</xdr:rowOff>
+      <xdr:rowOff>232200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -318,7 +581,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="770400" y="4677120"/>
-          <a:ext cx="1103400" cy="167760"/>
+          <a:ext cx="1103040" cy="167400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -367,9 +630,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>606960</xdr:colOff>
+      <xdr:colOff>606600</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>630720</xdr:rowOff>
+      <xdr:rowOff>630360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -379,7 +642,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="190800" y="5032080"/>
-          <a:ext cx="416160" cy="210960"/>
+          <a:ext cx="415800" cy="210600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -429,17 +692,18 @@
   </sheetPr>
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="24.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="59.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="68.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="6" style="0" width="24.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="63.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="75.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="57.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="7" style="0" width="24.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -502,193 +766,329 @@
       <c r="E5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="4"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="F8" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
+      <c r="D9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="131.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="4"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="116.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="155.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>6</v>
+        <v>28</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="78.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="D13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="75.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="104.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="110.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="103.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="98.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="96.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="84.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="4"/>
+      <c r="A21" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="181.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="7"/>
@@ -696,7 +1096,7 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
-      <c r="F23" s="4"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="7"/>
@@ -704,7 +1104,7 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="4"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="7"/>
@@ -712,119 +1112,119 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="4"/>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
     </row>
     <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
     </row>
     <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
     </row>
     <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
     </row>
     <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
     </row>
     <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
     </row>
     <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
     </row>
     <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
     </row>
     <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
     </row>
     <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
     </row>
     <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
     </row>
     <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
     </row>
     <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
     </row>
     <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:E3"/>
     <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A9:E10"/>
-    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A10:F10"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
added max reward model saving
</commit_message>
<xml_diff>
--- a/trains_et_procedures.xlsx
+++ b/trains_et_procedures.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
   <si>
     <t xml:space="preserve">motion_imitation_base/ : architecture du réseau de neurones de l'article (commande avec prédiction motion capture comme référence)
 motion_imitation/ : architecture du réseau de neurones avec commande en vitesse (vitesse linéaire + angulaire)</t>
@@ -288,6 +289,85 @@
   </si>
   <si>
     <t xml:space="preserve">mpi_train.sh /sbatch_script – motion_imi.job : obs avec le yaw + commande changée : à la place de donner la commande en vitesse des vitesses angulaires (dr, dp, dy) on donne la position angulaire à rejoindre via un quaternion (qx,qy,qz,qw) : Décommenter fonction build_target_obs() ligne 266 de motion_imitation/envs/env_wrappers/imitation_task.py et commenter les deux autres (autres cas) + faire de meme pour la fonction get_target_obs_bounds() du meme fichier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajouter/Enlever l'observation (yaw, yawrate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/envs/env_builder.py : build_imitation_env() l. 97-98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fonction originale pour la construction de la commande du robot</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> motion_imitation/envs/env_wrappers/imitation_task.py : build_target_obs() l.299
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">
+Motion_imitation/envs/env_wrappers/imitation_task.py : build_target_obs() l.376</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">fonction pour la construction de la commande du robot en vitesses (vx, vy, vz, dr, dp, dy)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">motion_imitation/envs/env_wrappers/imitation_task.py : build_target_obs() l. 283
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">
+motion_imitation/envs/env_wrappers/imitation_task.py : build_target_obs() l. 361</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">fonction pour la construction de la commande du robot en vitesse linéaire + position angulaire de la base (vx, vy, vz, qx, qy, qz, qw)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/envs/env_wrappers/imitation_task.py : build_target_obs() l. 265
+motion_imitation/envs/env_wrappers/imitation_task.py : build_target_obs() l. 346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajouter/Enlever le bruit sur la commande. Décommenter la bonne ligne pour une commande (vx, vy, vz, dr, dp, dy) ou une commande (vx, vy, vz, qx, qy, qz, qw)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/envs/env_wrappers/imitation_wrapper_env.py : build_imitation_env() l. 105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajouter/enlever/réglage des escaliers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/envs/locomotion_gym_env.py : reset() l. 269</t>
+  </si>
+  <si>
+    <t xml:space="preserve">création d'un terrain accidenté/escarpé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/envs/locomotion_gym_env.py : reset() l. 237</t>
   </si>
 </sst>
 </file>
@@ -395,7 +475,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -446,6 +526,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -685,6 +773,381 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>61560</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>443520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>35640</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1611720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4120920" y="443520"/>
+          <a:ext cx="12739680" cy="1168200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>48960</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>275760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7192080</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2161440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4108320" y="2181960"/>
+          <a:ext cx="7143120" cy="1885680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>61200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>259920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>10371240</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3110040</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4120560" y="6725160"/>
+          <a:ext cx="10310040" cy="2850120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12240</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>303120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>11165760</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3326400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 5" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4071600" y="13478400"/>
+          <a:ext cx="11153520" cy="3023280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>49320</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3684240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6485400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>6248160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 6" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4108680" y="16859520"/>
+          <a:ext cx="6436080" cy="2563920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>37080</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3443040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6184800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>6092640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Image 7" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId6"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4096440" y="9908280"/>
+          <a:ext cx="6147720" cy="2649600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>98280</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2550600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6329160</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4426920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Image 8" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId7"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4157640" y="4456800"/>
+          <a:ext cx="6230880" cy="1876320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>232920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>10740240</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>3606120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Image 9" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId8"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4071960" y="19680840"/>
+          <a:ext cx="10727640" cy="3373200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>61200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>426600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>11650680</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>4214160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Image 10" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId9"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4120560" y="23519520"/>
+          <a:ext cx="11589480" cy="3787560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>48960</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>569520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>8325720</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>6600600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Image 11" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId10"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4108320" y="27990000"/>
+          <a:ext cx="8276760" cy="6031080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -692,8 +1155,8 @@
   </sheetPr>
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B16" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -703,7 +1166,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="63.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="75.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="57.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="7" style="0" width="24.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="92.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="9" style="0" width="24.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1106,7 +1571,7 @@
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="62.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1235,4 +1700,192 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="180.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="0" width="21.77"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="150.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+    </row>
+    <row r="2" customFormat="false" ht="359" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="528.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="493.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" customFormat="false" ht="287" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" customFormat="false" ht="340.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="536.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="261.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="261.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="261.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new end eff sigmoid based reward function
</commit_message>
<xml_diff>
--- a/trains_et_procedures.xlsx
+++ b/trains_et_procedures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="116">
   <si>
     <t xml:space="preserve">motion_imitation_base/ : architecture du réseau de neurones de l'article (commande avec prédiction motion capture comme référence)
 motion_imitation/ : architecture du réseau de neurones avec commande en vitesse (vitesse linéaire + angulaire)</t>
@@ -209,8 +209,32 @@
     <t xml:space="preserve">model_saves/hard_ref_yaw/</t>
   </si>
   <si>
-    <t xml:space="preserve">marche avec une référence compliquée pour apprendre la marche arrière + changement de directions.
-Version avec la mesure du yaw et yaw rate en entrée du réseau. Mauvais résultats.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">marche avec une référence compliquée pour apprendre la marche arrière + changement de directions.
+Version avec la mesure du yaw et yaw rate en entrée du réseau. </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Mauvais résultats</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">test.sh avec l'observation avec le yaw (r,p,y,dr,dp,dy) : Commenter motion_imitation/envs/env_builder.py ligne 98 et décommenter la ligne 97</t>
@@ -252,7 +276,34 @@
     <t xml:space="preserve">model_saves/zigzag_yaw/</t>
   </si>
   <si>
-    <t xml:space="preserve">marche en zigzag avec vitesse sur le yaw (cap changeant, pas de pas cotés). Mauvais résultats : marche quasi rectiligne, ne suit pas la référence qui marche en zigzagant du tout</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">marche en zigzag avec vitesse sur le yaw (cap changeant, pas de pas cotés). </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mauvais résultats </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">: marche quasi rectiligne, ne suit pas la référence qui marche en zigzagant du tout</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">static_turn</t>
@@ -264,7 +315,34 @@
     <t xml:space="preserve">model_saves/static_turn/</t>
   </si>
   <si>
-    <t xml:space="preserve">marche où le robot tourne autour de lui-même (à partir d'un fichier .txt de ref custom). Mauvais résultats : robot reste immobile</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">marche où le robot tourne autour de lui-même – droite puis gauche (à partir d'un fichier .txt de ref custom). </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mauvais résultats</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> : robot reste immobile</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">test.sh : obs avec le yaw</t>
@@ -282,13 +360,176 @@
     <t xml:space="preserve">model_saves/spin/</t>
   </si>
   <si>
-    <t xml:space="preserve">marche où le robot tourne (assez vite) autour de lui-même (fichier de ref txt non custom : déjà présent dans le git)</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">marche où le robot tourne (assez vite) autour de lui-même (fichier de ref txt non custom : déjà présent dans le git).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Bons résultats :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> le robot tourne bien rapidement dans une seule direction autour de lui-même.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">test.sh : obs avec le yaw + commande changée : à la place de donner la commande en vitesse des vitesses angulaires (dr, dp, dy) on donne la position angulaire à rejoindre via un quaternion (qx,qy,qz,qw) : Décommenter fonction build_target_obs() ligne 266 de motion_imitation/envs/env_wrappers/imitation_task.py et commenter les deux autres (autres cas) + faire de meme pour la fonction get_target_obs_bounds() du meme fichier.</t>
   </si>
   <si>
     <t xml:space="preserve">mpi_train.sh /sbatch_script – motion_imi.job : obs avec le yaw + commande changée : à la place de donner la commande en vitesse des vitesses angulaires (dr, dp, dy) on donne la position angulaire à rejoindre via un quaternion (qx,qy,qz,qw) : Décommenter fonction build_target_obs() ligne 266 de motion_imitation/envs/env_wrappers/imitation_task.py et commenter les deux autres (autres cas) + faire de meme pour la fonction get_target_obs_bounds() du meme fichier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/data/motions/data_train_14.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/static_turn_quater_input_failed/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">entrainement avec une référence (comportant des défauts) qui tourne autour d'elle même – droite puis gauche (plus vite, pas plus grands -&gt; allure plus différente que pour data_train_13.txt) et sans noise sur la commande pendant le train. </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mauvais résultats</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> : robot reste immobile.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">test.sh : obs avec le yaw (idem que le data_train_13) mais avec le fichier data_train_14. Input d'orientation : quaternion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">procédure (train) classique et enlever le noise, yaw obs + quaternion commande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/data/motions/data_train_18.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/static_turn_quater_data_18/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">entrainement avec référence corrigée (sans défauts) qui tourn autour d'elle même, sans noise + quaternion position pour la commande en orientation du robot. </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Résultats moyens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> : robot tourne autour de lui même mais piétine (pas d'allure de marche semblable à la référence).</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">test.sh : obs avec le yaw + quaternion pour la commande en orientation du robot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motion_imitation/data/motions/turn.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/base_turn_quater/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">entrainement avec référence "turn.txt" (fournie par le code originel de l'article). Pour vérifier que notre architecture permet d'apprendre à tourner à gauche puis à droite.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Résultats moyens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Roboto Mono"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> : robot tourne autour de lui même mais piétine (pas d'allure de marche semblable à la référence – moins que data_train_18).</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/stq_data_18_endeff_rew/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entrainement avec référence "data_train_18.txt". Reward modifié : si la différence de hauteur (z) entre le bout de la patte (end effector) de la simu et la réf est supérieur à 0.04 alors reward total = 0. C'est pour pénaliser grandement le non respect du mouvement des pattes dans le reward en espérant que le simu apprendra à mieux suivre l'allure de marche lorsque le robot tourne.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test.sh : yaw obs + quat cmd + reward end eff tweaké (commenter/décommenter l.579-581 – imitation_task.py : _calc_reward_end_effector())</t>
+  </si>
+  <si>
+    <t xml:space="preserve">procédure (train) classique et enlever le noise, yaw obs + 
+Quaternion commande + reward spécial end eff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/base_turn_quater_endeff_rew/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idem que pour l'entrainement ci dessus, à la différence qu'on lance le train avec la référence turn.txt issue du code originel de l'article</t>
   </si>
   <si>
     <t xml:space="preserve">Ajouter/Enlever l'observation (yaw, yawrate)</t>
@@ -377,7 +618,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -415,6 +656,19 @@
       <sz val="10"/>
       <name val="Roboto Mono"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Roboto Mono"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Roboto Mono"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -475,7 +729,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -526,6 +780,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -620,7 +878,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2955960</xdr:colOff>
+      <xdr:colOff>2419560</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>2502720</xdr:rowOff>
     </xdr:to>
@@ -1153,19 +1411,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B16" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="24.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="63.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="75.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="57.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="63.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="92.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="9" style="0" width="24.53"/>
@@ -1555,134 +1814,276 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="84.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="93.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" customFormat="false" ht="62.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="108.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="98.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="83.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
+      <c r="B27" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1709,7 +2110,7 @@
   </sheetPr>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1722,10 +2123,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="150.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>85</v>
+        <v>102</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
@@ -1739,10 +2140,10 @@
     </row>
     <row r="2" customFormat="false" ht="359" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>87</v>
+        <v>104</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -1756,10 +2157,10 @@
     </row>
     <row r="3" customFormat="false" ht="528.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>89</v>
+        <v>106</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1773,10 +2174,10 @@
     </row>
     <row r="4" customFormat="false" ht="493.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>91</v>
+        <v>108</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>109</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1790,10 +2191,10 @@
     </row>
     <row r="5" customFormat="false" ht="287" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>93</v>
+        <v>110</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -1807,10 +2208,10 @@
     </row>
     <row r="6" customFormat="false" ht="340.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>95</v>
+        <v>112</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -1824,10 +2225,10 @@
     </row>
     <row r="7" customFormat="false" ht="536.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>97</v>
+        <v>114</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>115</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1841,7 +2242,7 @@
     </row>
     <row r="8" customFormat="false" ht="261.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
-      <c r="B8" s="13"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -1854,7 +2255,7 @@
     </row>
     <row r="9" customFormat="false" ht="261.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7"/>
-      <c r="B9" s="13"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1867,7 +2268,7 @@
     </row>
     <row r="10" customFormat="false" ht="261.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
-      <c r="B10" s="13"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>

</xml_diff>

<commit_message>
changed to data train 19 and increased end eff subreward's weight
</commit_message>
<xml_diff>
--- a/trains_et_procedures.xlsx
+++ b/trains_et_procedures.xlsx
@@ -21,10 +21,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="122">
   <si>
     <t xml:space="preserve">motion_imitation_base/ : architecture du réseau de neurones de l'article (commande avec prédiction motion capture comme référence)
-motion_imitation/ : architecture du réseau de neurones avec commande en vitesse (vitesse linéaire + angulaire)</t>
+motion_imitation/ : architecture du réseau de neurones avec commande en vitesse (vitesse linéaire + angulaire)
+Les différentes fonctions de reward utilisées sont dans reward_funcs.txt</t>
   </si>
   <si>
     <t xml:space="preserve">Fichier de référence</t>
@@ -214,6 +215,7 @@
         <sz val="10"/>
         <rFont val="Roboto Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">marche avec une référence compliquée pour apprendre la marche arrière + changement de directions.
 Version avec la mesure du yaw et yaw rate en entrée du réseau. </t>
@@ -224,6 +226,7 @@
         <sz val="10"/>
         <rFont val="Roboto Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mauvais résultats</t>
     </r>
@@ -232,6 +235,7 @@
         <sz val="10"/>
         <rFont val="Roboto Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
@@ -500,6 +504,7 @@
         <sz val="10"/>
         <rFont val="Roboto Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Résultats moyens</t>
     </r>
@@ -508,12 +513,13 @@
         <sz val="10"/>
         <rFont val="Roboto Mono"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> : robot tourne autour de lui même mais piétine (pas d'allure de marche semblable à la référence – moins que data_train_18).</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">model_saves/stq_data_18_endeff_rew/</t>
+    <t xml:space="preserve">model_saves/stq_data_18_endeff_rew_1/</t>
   </si>
   <si>
     <t xml:space="preserve">entrainement avec référence "data_train_18.txt". Reward modifié : si la différence de hauteur (z) entre le bout de la patte (end effector) de la simu et la réf est supérieur à 0.04 alors reward total = 0. C'est pour pénaliser grandement le non respect du mouvement des pattes dans le reward en espérant que le simu apprendra à mieux suivre l'allure de marche lorsque le robot tourne.</t>
@@ -532,6 +538,25 @@
     <t xml:space="preserve">idem que pour l'entrainement ci dessus, à la différence qu'on lance le train avec la référence turn.txt issue du code originel de l'article</t>
   </si>
   <si>
+    <t xml:space="preserve">model_saves/stq_data_18_endeff_rew_2/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entrainement avec référence "data_train_18.txt". Reward modifié : si la différence de hauteur (z) entre le bout de la patte (end effector) de la simu et la réf est supérieur à 0.02 alors reward total = 0. C'est pour pénaliser grandement le non respect du mouvement des pattes dans le reward en espérant que le simu apprendra à mieux suivre l'allure de marche lorsque le robot tourne.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model_saves/stq_d18_sigrew/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entrainement avec le sous reward du end effector remplacé par une fonction de type sigmoide : pour permettre les rewards négatifs et rendre l'erreur sur les end effectors plus impactante sur le reward global</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test.sh : yaw obs + quat cmd + reward end eff sigmoide (commenter/décommenter la bonne fonction – imitation_task.py : _calc_reward_end_effector()) -&gt; principalement si on veut plot le bon reward lors d'un test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">procédure (train) classique et enlever le noise, yaw obs + 
+Quaternion commande + reward spécial end eff sigmoide</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ajouter/Enlever l'observation (yaw, yawrate)</t>
   </si>
   <si>
@@ -541,49 +566,15 @@
     <t xml:space="preserve">fonction originale pour la construction de la commande du robot</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Roboto Mono"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> motion_imitation/envs/env_wrappers/imitation_task.py : build_target_obs() l.299
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Roboto Mono"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t xml:space="preserve"> motion_imitation/envs/env_wrappers/imitation_task.py : build_target_obs() l.299
 Motion_imitation/envs/env_wrappers/imitation_task.py : build_target_obs() l.376</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">fonction pour la construction de la commande du robot en vitesses (vx, vy, vz, dr, dp, dy)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Roboto Mono"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">motion_imitation/envs/env_wrappers/imitation_task.py : build_target_obs() l. 283
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Roboto Mono"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t xml:space="preserve">motion_imitation/envs/env_wrappers/imitation_task.py : build_target_obs() l. 283
 motion_imitation/envs/env_wrappers/imitation_task.py : build_target_obs() l. 361</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">fonction pour la construction de la commande du robot en vitesse linéaire + position angulaire de la base (vx, vy, vz, qx, qy, qz, qw)</t>
@@ -618,7 +609,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -653,22 +644,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Roboto Mono"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Roboto Mono"/>
-      <family val="0"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Roboto Mono"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Roboto Mono"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -729,7 +714,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -762,19 +747,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -782,15 +759,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -878,9 +855,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2419560</xdr:colOff>
+      <xdr:colOff>2419200</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>2502720</xdr:rowOff>
+      <xdr:rowOff>2502360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -894,7 +871,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="2154600"/>
-          <a:ext cx="12816720" cy="2260440"/>
+          <a:ext cx="12816360" cy="2260080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -915,9 +892,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1873440</xdr:colOff>
+      <xdr:colOff>1873080</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>232200</xdr:rowOff>
+      <xdr:rowOff>231840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -927,7 +904,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="770400" y="4677120"/>
-          <a:ext cx="1103040" cy="167400"/>
+          <a:ext cx="1102680" cy="167040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -976,9 +953,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>606600</xdr:colOff>
+      <xdr:colOff>606240</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>630360</xdr:rowOff>
+      <xdr:rowOff>630000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -988,7 +965,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="190800" y="5032080"/>
-          <a:ext cx="415800" cy="210600"/>
+          <a:ext cx="415440" cy="210240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1042,9 +1019,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>35640</xdr:colOff>
+      <xdr:colOff>35280</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1611720</xdr:rowOff>
+      <xdr:rowOff>1611360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1057,8 +1034,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4120920" y="443520"/>
-          <a:ext cx="12739680" cy="1168200"/>
+          <a:off x="4121640" y="443520"/>
+          <a:ext cx="12738600" cy="1167840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1079,9 +1056,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>7192080</xdr:colOff>
+      <xdr:colOff>7191720</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>2161440</xdr:rowOff>
+      <xdr:rowOff>2161080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1094,8 +1071,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4108320" y="2181960"/>
-          <a:ext cx="7143120" cy="1885680"/>
+          <a:off x="4109040" y="2181960"/>
+          <a:ext cx="7142760" cy="1885320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1116,9 +1093,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>10371240</xdr:colOff>
+      <xdr:colOff>10370880</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>3110040</xdr:rowOff>
+      <xdr:rowOff>3109680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1131,8 +1108,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4120560" y="6725160"/>
-          <a:ext cx="10310040" cy="2850120"/>
+          <a:off x="4121280" y="6725160"/>
+          <a:ext cx="10309680" cy="2849760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1153,9 +1130,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>11165760</xdr:colOff>
+      <xdr:colOff>11165400</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>3326400</xdr:rowOff>
+      <xdr:rowOff>3326040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1168,8 +1145,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4071600" y="13478400"/>
-          <a:ext cx="11153520" cy="3023280"/>
+          <a:off x="4072320" y="13478400"/>
+          <a:ext cx="11153160" cy="3022920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1190,9 +1167,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>6485400</xdr:colOff>
+      <xdr:colOff>6485040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>6248160</xdr:rowOff>
+      <xdr:rowOff>6247800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1205,8 +1182,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4108680" y="16859520"/>
-          <a:ext cx="6436080" cy="2563920"/>
+          <a:off x="4109400" y="16859520"/>
+          <a:ext cx="6435720" cy="2563560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1227,9 +1204,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>6184800</xdr:colOff>
+      <xdr:colOff>6184440</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>6092640</xdr:rowOff>
+      <xdr:rowOff>6092280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1242,8 +1219,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4096440" y="9908280"/>
-          <a:ext cx="6147720" cy="2649600"/>
+          <a:off x="4097160" y="9908280"/>
+          <a:ext cx="6147360" cy="2649240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1264,9 +1241,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>6329160</xdr:colOff>
+      <xdr:colOff>6328800</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>4426920</xdr:rowOff>
+      <xdr:rowOff>4426560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1279,8 +1256,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4157640" y="4456800"/>
-          <a:ext cx="6230880" cy="1876320"/>
+          <a:off x="4158360" y="4456800"/>
+          <a:ext cx="6230520" cy="1875960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1301,9 +1278,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>10740240</xdr:colOff>
+      <xdr:colOff>10739880</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>3606120</xdr:rowOff>
+      <xdr:rowOff>3605760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1316,8 +1293,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4071960" y="19680840"/>
-          <a:ext cx="10727640" cy="3373200"/>
+          <a:off x="4072680" y="19680840"/>
+          <a:ext cx="10727280" cy="3372840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1338,9 +1315,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>11650680</xdr:colOff>
+      <xdr:colOff>11650320</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>4214160</xdr:rowOff>
+      <xdr:rowOff>4213800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1353,8 +1330,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4120560" y="23519520"/>
-          <a:ext cx="11589480" cy="3787560"/>
+          <a:off x="4121280" y="23519520"/>
+          <a:ext cx="11589120" cy="3787200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1375,9 +1352,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>8325720</xdr:colOff>
+      <xdr:colOff>8325360</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>6600600</xdr:rowOff>
+      <xdr:rowOff>6600240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1390,8 +1367,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4108320" y="27990000"/>
-          <a:ext cx="8276760" cy="6031080"/>
+          <a:off x="4109040" y="27990000"/>
+          <a:ext cx="8276400" cy="6030720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1413,11 +1390,11 @@
   </sheetPr>
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B22" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.53"/>
@@ -1598,7 +1575,7 @@
       <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -1618,7 +1595,7 @@
       <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -1635,22 +1612,22 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="75.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1675,42 +1652,42 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="110.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="103.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="9" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1718,7 +1695,7 @@
       <c r="A18" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -1730,67 +1707,67 @@
       <c r="E18" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="96.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="9" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="84.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="9" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="59.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1798,7 +1775,7 @@
       <c r="A22" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="7" t="s">
         <v>79</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -1810,25 +1787,25 @@
       <c r="E22" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="7" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="84.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="7"/>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1861,15 +1838,15 @@
       <c r="D25" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="7" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="98.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="7" t="s">
         <v>89</v>
       </c>
@@ -1887,7 +1864,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="83.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="7" t="s">
         <v>93</v>
       </c>
@@ -1897,31 +1874,51 @@
       <c r="D27" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F27" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+    <row r="28" customFormat="false" ht="98.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10"/>
+      <c r="B28" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="56.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10"/>
+      <c r="B29" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12"/>
+      <c r="A30" s="10"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1929,7 +1926,7 @@
       <c r="F30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1937,7 +1934,7 @@
       <c r="F31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1945,7 +1942,7 @@
       <c r="F32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1953,7 +1950,7 @@
       <c r="F33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12"/>
+      <c r="A34" s="10"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -1961,7 +1958,7 @@
       <c r="F34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1969,7 +1966,7 @@
       <c r="F35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1977,7 +1974,7 @@
       <c r="F36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -1985,7 +1982,7 @@
       <c r="F37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -1993,7 +1990,7 @@
       <c r="F38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -2001,7 +1998,7 @@
       <c r="F39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12"/>
+      <c r="A40" s="10"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -2065,25 +2062,25 @@
       <c r="F48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
     </row>
     <row r="50" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="13"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
     </row>
     <row r="51" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2114,7 +2111,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="180.91"/>
@@ -2123,10 +2120,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="150.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>103</v>
+        <v>108</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
@@ -2140,10 +2137,10 @@
     </row>
     <row r="2" customFormat="false" ht="359" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>105</v>
+        <v>110</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2157,10 +2154,10 @@
     </row>
     <row r="3" customFormat="false" ht="528.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>107</v>
+        <v>112</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -2173,11 +2170,11 @@
       <c r="K3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="493.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>109</v>
+      <c r="A4" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -2191,10 +2188,10 @@
     </row>
     <row r="5" customFormat="false" ht="287" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>111</v>
+        <v>116</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>117</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -2208,10 +2205,10 @@
     </row>
     <row r="6" customFormat="false" ht="340.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>113</v>
+        <v>118</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -2225,10 +2222,10 @@
     </row>
     <row r="7" customFormat="false" ht="536.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>115</v>
+        <v>120</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -2242,7 +2239,7 @@
     </row>
     <row r="8" customFormat="false" ht="261.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
-      <c r="B8" s="14"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -2255,7 +2252,7 @@
     </row>
     <row r="9" customFormat="false" ht="261.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7"/>
-      <c r="B9" s="14"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -2268,7 +2265,7 @@
     </row>
     <row r="10" customFormat="false" ht="261.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
-      <c r="B10" s="14"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>

</xml_diff>